<commit_message>
Updated with Excel Sample
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared_TC_Projects\Demo_CI_Suite\Bearstore_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KMJ\TC_Head_Start_Suite\VET_JavaScript_Project\Data_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC9D242-D0DE-4A6E-A3FB-AE91C2154CEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A95E181C-BDD5-4F84-BE6B-776E1060E8A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="10920" xr2:uid="{084FFFA1-4D60-4752-B414-257B00A5D176}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contact_Information" sheetId="1" r:id="rId1"/>
+    <sheet name="Captured_Values" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="true"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -130,6 +131,24 @@
   </si>
   <si>
     <t>dan@smartbear.com</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
 </sst>
 </file>
@@ -167,7 +186,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,18 +503,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25349621-2914-4FB2-82D4-8E41E1C25A8A}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="true" customWidth="true"/>
+    <col min="2" max="2" width="22.5703125" bestFit="true" customWidth="true"/>
+    <col min="3" max="3" width="25.5703125" bestFit="true" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -517,7 +536,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -528,7 +547,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -539,7 +558,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -550,7 +569,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -561,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -572,7 +591,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -583,7 +602,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -594,7 +613,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -605,7 +624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -614,6 +633,65 @@
       </c>
       <c r="C11" s="1" t="s">
         <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="false" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="true"/>
+    <col min="2" max="2" width="61.5703125" customWidth="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" customHeight="true" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>123456789</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>123456789</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>123456789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>123456789</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed Visualizer files and other minor tweaks
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -651,7 +660,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -727,6 +736,30 @@
         <v>40</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9">
+        <v>123456789</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>123456789</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>123456789</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added Custom Warning message for tests that have failed often
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -660,7 +669,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -760,6 +769,30 @@
         <v>43</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12">
+        <v>123456789</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>123456789</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>123456789</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with various things
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -669,7 +678,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -793,6 +802,30 @@
         <v>46</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15">
+        <v>123456789</v>
+      </c>
+      <c r="B15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>123456789</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>123456789</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated tests to get to 100% Pass
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,33 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -687,7 +714,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -859,6 +886,78 @@
         <v>52</v>
       </c>
     </row>
+    <row r="21">
+      <c r="A21">
+        <v>123456789</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>123456789</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>123456789</v>
+      </c>
+      <c r="B23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>123456789</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>123456789</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>123456789</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>123456789</v>
+      </c>
+      <c r="B27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>123456789</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>123456789</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Nothing to see here, move along
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -732,7 +741,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -1024,6 +1033,30 @@
         <v>67</v>
       </c>
     </row>
+    <row r="36">
+      <c r="A36">
+        <v>123456789</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>123456789</v>
+      </c>
+      <c r="B37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>123456789</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to Projects with common settings (Minimize TC on playback and stop on unexpected windows) Plus other minor updates
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,42 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -741,7 +777,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -1057,6 +1093,102 @@
         <v>70</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39">
+        <v>123456789</v>
+      </c>
+      <c r="B39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>123456789</v>
+      </c>
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>123456789</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>123456789</v>
+      </c>
+      <c r="B42" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>123456789</v>
+      </c>
+      <c r="B43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>123456789</v>
+      </c>
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>123456789</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>123456789</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>123456789</v>
+      </c>
+      <c r="B47" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>123456789</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>123456789</v>
+      </c>
+      <c r="B49" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>123456789</v>
+      </c>
+      <c r="B50" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Scripts for testing browser loops
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,69 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -828,7 +891,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:B88"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -1376,6 +1439,174 @@
         <v>99</v>
       </c>
     </row>
+    <row r="68">
+      <c r="A68">
+        <v>123456789</v>
+      </c>
+      <c r="B68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>123456789</v>
+      </c>
+      <c r="B69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
+        <v>123456789</v>
+      </c>
+      <c r="B70" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>123456789</v>
+      </c>
+      <c r="B71" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>123456789</v>
+      </c>
+      <c r="B72" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>123456789</v>
+      </c>
+      <c r="B73" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74">
+        <v>123456789</v>
+      </c>
+      <c r="B74" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75">
+        <v>123456789</v>
+      </c>
+      <c r="B75" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>123456789</v>
+      </c>
+      <c r="B76" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77">
+        <v>123456789</v>
+      </c>
+      <c r="B77" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>123456789</v>
+      </c>
+      <c r="B78" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>123456789</v>
+      </c>
+      <c r="B79" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80">
+        <v>123456789</v>
+      </c>
+      <c r="B80" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81">
+        <v>123456789</v>
+      </c>
+      <c r="B81" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82">
+        <v>123456789</v>
+      </c>
+      <c r="B82" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83">
+        <v>123456789</v>
+      </c>
+      <c r="B83" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84">
+        <v>123456789</v>
+      </c>
+      <c r="B84" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85">
+        <v>123456789</v>
+      </c>
+      <c r="B85" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86">
+        <v>123456789</v>
+      </c>
+      <c r="B86" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87">
+        <v>123456789</v>
+      </c>
+      <c r="B87" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88">
+        <v>123456789</v>
+      </c>
+      <c r="B88" t="s">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates of log loops
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,21 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -891,7 +906,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B88"/>
+  <dimension ref="A1:B93"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -1607,6 +1622,46 @@
         <v>120</v>
       </c>
     </row>
+    <row r="89">
+      <c r="A89">
+        <v>123456789</v>
+      </c>
+      <c r="B89" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90">
+        <v>123456789</v>
+      </c>
+      <c r="B90" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91">
+        <v>123456789</v>
+      </c>
+      <c r="B91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92">
+        <v>0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93">
+        <v>123456789</v>
+      </c>
+      <c r="B93" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to get all project execution plans to 100%
</commit_message>
<xml_diff>
--- a/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
+++ b/VET_JavaScript_Project/Data_Files/Contact_List.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -137,6 +137,33 @@
   </si>
   <si>
     <t>Text1</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
+  </si>
+  <si>
+    <t>Real Programmers Count 0123456789 From Zero</t>
   </si>
   <si>
     <t>Real Programmers Count 0123456789 From Zero</t>
@@ -906,7 +933,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B21B73F3-C035-465C-8561-7E8EEB54B5CA}">
-  <dimension ref="A1:B93"/>
+  <dimension ref="A1:B102"/>
   <sheetViews>
     <sheetView tabSelected="false" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD8"/>
@@ -1662,6 +1689,78 @@
         <v>125</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94">
+        <v>123456789</v>
+      </c>
+      <c r="B94" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95">
+        <v>123456789</v>
+      </c>
+      <c r="B95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96">
+        <v>123456789</v>
+      </c>
+      <c r="B96" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97">
+        <v>123456789</v>
+      </c>
+      <c r="B97" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98">
+        <v>123456789</v>
+      </c>
+      <c r="B98" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99">
+        <v>123456789</v>
+      </c>
+      <c r="B99" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100">
+        <v>123456789</v>
+      </c>
+      <c r="B100" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101">
+        <v>123456789</v>
+      </c>
+      <c r="B101" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102">
+        <v>123456789</v>
+      </c>
+      <c r="B102" t="s">
+        <v>134</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>